<commit_message>
registro, login e inicio mejorado y Registro con estilos
</commit_message>
<xml_diff>
--- a/OrganizaciónE3E4.xlsx
+++ b/OrganizaciónE3E4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BA1375-D7C6-4539-B5FC-D7C96DDBDBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1AEC4-3657-406C-AC34-0F6D2F4C0A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83273B90-A93D-4C70-97AC-CC5DB7764BD8}"/>
   </bookViews>
@@ -722,7 +722,7 @@
   <dimension ref="B6:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel organización E3-E4 actualizado
</commit_message>
<xml_diff>
--- a/OrganizaciónE3E4.xlsx
+++ b/OrganizaciónE3E4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\asignaturas\2\Web\Proyectos2025\ProyectoWeb2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\E2_IW_2025\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1AEC4-3657-406C-AC34-0F6D2F4C0A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8B1A2-7372-4A1F-BB6B-BDDBB4328F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83273B90-A93D-4C70-97AC-CC5DB7764BD8}"/>
+    <workbookView xWindow="7200" yWindow="30" windowWidth="21600" windowHeight="11295" xr2:uid="{83273B90-A93D-4C70-97AC-CC5DB7764BD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Desarrollo Tecnico (3)</t>
   </si>
@@ -721,15 +721,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D6CDB-C808-4446-9D76-8250F2A4CABA}">
   <dimension ref="B6:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="73.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -883,8 +883,12 @@
       <c r="D19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
+      <c r="E19" s="27">
+        <v>45789</v>
+      </c>
+      <c r="F19" s="28">
+        <v>45791</v>
+      </c>
     </row>
     <row r="20" spans="2:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
@@ -917,7 +921,9 @@
       <c r="C22" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="E22" s="33"/>
       <c r="F22" s="34"/>
     </row>
@@ -937,8 +943,12 @@
       <c r="C24" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="27"/>
+      <c r="D24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="27">
+        <v>45793</v>
+      </c>
       <c r="F24" s="28"/>
     </row>
     <row r="25" spans="2:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -948,7 +958,9 @@
       <c r="C25" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="E25" s="35"/>
       <c r="F25" s="36"/>
     </row>

</xml_diff>

<commit_message>
*Actualización de la documentación de Excel en un solo fichero siguiendo instrucciones *presentacionVideo.txt con los enlaces a la presentacion y al video (E4)
</commit_message>
<xml_diff>
--- a/OrganizaciónE3E4.xlsx
+++ b/OrganizaciónE3E4.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\E2_IW_2025\ProyectoWeb2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\proyectoColaborativo\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8B1A2-7372-4A1F-BB6B-BDDBB4328F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D9B02B-7226-4034-8B35-19A359EB49C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="30" windowWidth="21600" windowHeight="11295" xr2:uid="{83273B90-A93D-4C70-97AC-CC5DB7764BD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{83273B90-A93D-4C70-97AC-CC5DB7764BD8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="E3+E4" sheetId="1" r:id="rId1"/>
+    <sheet name="E2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>Desarrollo Tecnico (3)</t>
   </si>
@@ -142,12 +143,117 @@
   <si>
     <t>Gaizka</t>
   </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Fecha fin e inicio</t>
+  </si>
+  <si>
+    <t>Creacion proyecto, funciones listar y detalles</t>
+  </si>
+  <si>
+    <t>Detalles arreglado, creación medio hecho</t>
+  </si>
+  <si>
+    <t>Crear con formularios: Proyecto, Tarea, Empleado</t>
+  </si>
+  <si>
+    <t>Estilos: Base, Create y Formularios</t>
+  </si>
+  <si>
+    <t>Update hecho</t>
+  </si>
+  <si>
+    <t>Eliminar con botón desde detalles: Proyecto, Tarea, Empleado</t>
+  </si>
+  <si>
+    <t>Estilos: Detalles de proyectos, empleados y tareas</t>
+  </si>
+  <si>
+    <t>Creación del modelo Herramientas, todas las views(herramienta)</t>
+  </si>
+  <si>
+    <t>Templates(herramientas) y formulario (herramientas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Footer hecho</t>
+  </si>
+  <si>
+    <t>Modelo tarea arreglado</t>
+  </si>
+  <si>
+    <t>Footer con últimos empleados, herramientas, tareas, empleados (extra)</t>
+  </si>
+  <si>
+    <t>Estilos: Logos footer</t>
+  </si>
+  <si>
+    <t>Cambios en views.py</t>
+  </si>
+  <si>
+    <t>Modificación del Footer vista detalle</t>
+  </si>
+  <si>
+    <t>Segunda linea de menu horizontal, botón de editar en los detalles</t>
+  </si>
+  <si>
+    <t>Modificación de templates, recoger ultimos 3 empleados (list,create,detail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultimos tres en body, estilos de crear </t>
+  </si>
+  <si>
+    <t>Estilos: Ultimos empleados, proyectos, tareas y herramientas</t>
+  </si>
+  <si>
+    <t>Boton eliminar y editar en "Detalles"</t>
+  </si>
+  <si>
+    <t>Extra: Tareas "en proceso" del listado de tareas</t>
+  </si>
+  <si>
+    <t>Añadir modelo herramienta a adminDjango</t>
+  </si>
+  <si>
+    <t>Extra: Herramientas con baja disponibilidad del listado de herramientas</t>
+  </si>
+  <si>
+    <t>Extra: Proyectos de alto presupuesto del listado de proyectos</t>
+  </si>
+  <si>
+    <t>Mejora de modelos, modificación de campos y actualización templates</t>
+  </si>
+  <si>
+    <t>Extra: Empleados no disponibles del listado de empleados</t>
+  </si>
+  <si>
+    <t>Correccion y limpieza en codigo</t>
+  </si>
+  <si>
+    <t>Actualización de los registros de la BD</t>
+  </si>
+  <si>
+    <t>Mostrar las herramientas por tarea (many to many)</t>
+  </si>
+  <si>
+    <t>Esquema entidad relación</t>
+  </si>
+  <si>
+    <t>Trabajos realizados por cada miembro del equipo en orden cronológico</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +263,28 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -337,10 +465,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -405,11 +534,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -420,6 +577,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86AB4A26-C9D2-4969-BCE5-AC3483318724}" name="Tabla1" displayName="Tabla1" ref="A2:C33" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A2:C33" xr:uid="{86AB4A26-C9D2-4969-BCE5-AC3483318724}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{33FD7FD4-CFD2-4204-9CB1-8FA76A586348}" name="Alumno"/>
+    <tableColumn id="2" xr3:uid="{E9DAA4FB-2B98-49BB-9109-4C31ED0765B2}" name="Tarea"/>
+    <tableColumn id="3" xr3:uid="{C2441899-9B68-432A-94F3-EC4D7F4647E8}" name="Fecha fin e inicio" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -719,21 +888,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D6CDB-C808-4446-9D76-8250F2A4CABA}">
-  <dimension ref="B6:F25"/>
+  <dimension ref="B6:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="53" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
@@ -742,7 +911,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -759,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>21</v>
       </c>
@@ -768,7 +937,7 @@
       <c r="E9" s="21"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="10">
         <v>2</v>
       </c>
@@ -781,20 +950,17 @@
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
     </row>
-    <row r="11" spans="2:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
         <v>2</v>
       </c>
@@ -807,7 +973,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
     </row>
-    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>2</v>
       </c>
@@ -817,20 +983,18 @@
       <c r="E13" s="29"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
         <v>1</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="27"/>
       <c r="F14" s="28"/>
     </row>
-    <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>1</v>
       </c>
@@ -840,7 +1004,7 @@
       <c r="E15" s="29"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10">
         <v>1</v>
       </c>
@@ -851,7 +1015,7 @@
       <c r="E16" s="27"/>
       <c r="F16" s="28"/>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="25" t="s">
         <v>17</v>
       </c>
@@ -860,7 +1024,7 @@
       <c r="E17" s="31"/>
       <c r="F17" s="32"/>
     </row>
-    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="15">
         <v>1</v>
       </c>
@@ -868,12 +1032,14 @@
         <v>13</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="33"/>
+        <v>23</v>
+      </c>
+      <c r="E18" s="33">
+        <v>45797</v>
+      </c>
       <c r="F18" s="34"/>
     </row>
-    <row r="19" spans="2:6" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="158.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <v>1</v>
       </c>
@@ -890,7 +1056,7 @@
         <v>45791</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15">
         <v>1</v>
       </c>
@@ -898,12 +1064,14 @@
         <v>22</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="33"/>
+        <v>23</v>
+      </c>
+      <c r="E20" s="33">
+        <v>45797</v>
+      </c>
       <c r="F20" s="34"/>
     </row>
-    <row r="21" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>1</v>
       </c>
@@ -914,7 +1082,7 @@
       <c r="E21" s="27"/>
       <c r="F21" s="28"/>
     </row>
-    <row r="22" spans="2:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="15">
         <v>1</v>
       </c>
@@ -927,7 +1095,7 @@
       <c r="E22" s="33"/>
       <c r="F22" s="34"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="24" t="s">
         <v>18</v>
       </c>
@@ -936,9 +1104,9 @@
       <c r="E23" s="31"/>
       <c r="F23" s="32"/>
     </row>
-    <row r="24" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B24" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>19</v>
@@ -951,21 +1119,400 @@
       </c>
       <c r="F24" s="28"/>
     </row>
-    <row r="25" spans="2:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>24</v>
-      </c>
+      <c r="D25" s="19"/>
       <c r="E25" s="35"/>
       <c r="F25" s="36"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CF0CD5-4BDD-4119-B06B-A8654105D2DA}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="70.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="39">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="39">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="39">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="39">
+        <v>45767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="39">
+        <v>45767</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="39">
+        <v>45767</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="39">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="39">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="39">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="39">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="39">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="39">
+        <v>45774</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="39">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="39">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="39">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="39">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="39">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="39">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="39">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="39">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="39">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="39">
+        <v>45780</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="39">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="41">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="41">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="41">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="39">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="39">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="39">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="39">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="39">
+        <v>45784</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Añadir estilos (styles.css) a los botones de aumentar/dismuir tamaño de elementos tipo text
Actualizacion Excel OrganizacionE3E4
</commit_message>
<xml_diff>
--- a/OrganizaciónE3E4.xlsx
+++ b/OrganizaciónE3E4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hezitzaile\Desktop\proyectoColaborativo\ProyectoWeb2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D9B02B-7226-4034-8B35-19A359EB49C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625A4E4A-C557-4907-BDF4-18747D506B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{83273B90-A93D-4C70-97AC-CC5DB7764BD8}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="E2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Desarrollo Tecnico (3)</t>
   </si>
@@ -890,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D6CDB-C808-4446-9D76-8250F2A4CABA}">
   <dimension ref="B6:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="53" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,12 +1064,8 @@
       <c r="C20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="33">
-        <v>45797</v>
-      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="34"/>
     </row>
     <row r="21" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>